<commit_message>
New framework for restapi
</commit_message>
<xml_diff>
--- a/ProjectDocuments/TimeSheets/AramTimeSheet.xlsx
+++ b/ProjectDocuments/TimeSheets/AramTimeSheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyProg\UniServerZ\www\SclProj\ProjectDocuments\TimeSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyProg\UniServerZ\www\OnlineShoppingProject\ProjectDocuments\TimeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B952723-6762-49AF-9ACB-950CE6FDCE13}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A06EA2D-2956-4A48-BFAC-B17D1E4B932A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>SYSTEM REQUREMENTS</t>
+  </si>
+  <si>
+    <t>21.3.2018</t>
+  </si>
+  <si>
+    <t>22.3.218</t>
+  </si>
+  <si>
+    <t>use case diagram</t>
   </si>
 </sst>
 </file>
@@ -397,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,6 +452,28 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>